<commit_message>
inclusão do readme e atualização planilha
</commit_message>
<xml_diff>
--- a/Planilhas Financeiras/DeclaracaoImpostoDeRenda/DeclaracaoImpostoDeRenda.xlsx
+++ b/Planilhas Financeiras/DeclaracaoImpostoDeRenda/DeclaracaoImpostoDeRenda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b052601145f258fa/Documentos/Jaidene/Cursos/Bootcamps/Simuladores_Excel/Planilhas Financeiras/DeclaracaoImpostoDeRenda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1935" documentId="8_{31041904-4F10-47C4-BD5F-AEF88D6EF06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B62F1D31-C502-458C-B7BB-C2054792F896}"/>
+  <xr:revisionPtr revIDLastSave="1938" documentId="8_{31041904-4F10-47C4-BD5F-AEF88D6EF06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7EE69E4-042A-4D7B-80C4-5F446C1B2484}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2565" yWindow="0" windowWidth="13995" windowHeight="10920" tabRatio="0" firstSheet="6" activeTab="6" xr2:uid="{119E6096-202F-4912-BDE6-3FEE23A5E77B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="0" xr2:uid="{119E6096-202F-4912-BDE6-3FEE23A5E77B}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMO" sheetId="2" r:id="rId1"/>
@@ -1280,9 +1280,6 @@
     <t>código</t>
   </si>
   <si>
-    <t>RESUMO</t>
-  </si>
-  <si>
     <t>Total de bens</t>
   </si>
   <si>
@@ -1296,6 +1293,9 @@
   </si>
   <si>
     <t>Valor total das informaçoes preenchidas</t>
+  </si>
+  <si>
+    <t>RESUMO GERAL</t>
   </si>
 </sst>
 </file>
@@ -9259,8 +9259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33476579-A4FD-4A7D-B5A9-8D7D75EDC9D3}">
   <dimension ref="A3:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -9279,19 +9279,19 @@
     <row r="4" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="3:4" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C6" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D6" s="30"/>
     </row>
     <row r="10" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D10" s="49">
         <f>SUM('BENS E DIREITOS'!D17,'BENS E DIREITOS'!D27,'BENS E DIREITOS'!D41,'BENS E DIREITOS'!D51,'BENS E DIREITOS'!D62,'BENS E DIREITOS'!D74)</f>
@@ -9308,7 +9308,7 @@
     </row>
     <row r="13" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="46" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D13" s="49">
         <f>SUM(DÍVIDAS!D15,DÍVIDAS!D24)</f>
@@ -9325,7 +9325,7 @@
     </row>
     <row r="16" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="46" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D16" s="49">
         <f>SUM(INFORMES!D12,INFORMES!D20,INFORMES!D28,INFORMES!D28,INFORMES!D36,)</f>
@@ -9345,7 +9345,7 @@
     </row>
     <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="46" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D19" s="49">
         <f>SUM('PGTO DEDUTÍVEIS'!D15,'PGTO DEDUTÍVEIS'!D24)</f>
@@ -13131,7 +13131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BFBFC7-D4E8-4B96-9FEB-A68195C1C26B}">
   <dimension ref="A3:D24"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">

</xml_diff>